<commit_message>
Added I2C LCD 16x2, button for TARA, and LED for indicating.
</commit_message>
<xml_diff>
--- a/venv/output.xlsx
+++ b/venv/output.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -53,18 +55,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +448,159 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2603.423076923077</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44260.53459715942</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2544.222222222222</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44260.54520345246</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2547.259259259259</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44260.54536520431</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44260.54552288155</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2550.148148148148</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44260.54738223815</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>44260.54751858036</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>68768.55555555556</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44260.55013614835</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2549.259259259259</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44260.57246532349</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-2521.814814814815</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44260.57480656946</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3446.444444444444</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44260.57951437631</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2549.074074074074</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>44260.57973993074</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6914.333333333333</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>44260.63564280069</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>-1.148148148148148</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>44260.63583176896</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2549.62962962963</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>44260.65864267803</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>19495.14814814815</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44260.73166254783</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2548.481481481481</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44260.73209902812</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>7505.089251804026</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44260.73854107285</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>15005.84884162552</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44260.7390276044</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2617.242688947968</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44260.74161344661</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>